<commit_message>
Logbook sections 14 and 15.
</commit_message>
<xml_diff>
--- a/Documentation/Logbook.xlsx
+++ b/Documentation/Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abram\Documents\IT\Major Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4F70A3-A9C8-4AC3-999F-47D83ACD29A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC236C2-2E56-4759-8898-180B8EB765F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A4DA64FF-B9B3-4233-BC20-5B0DAEA49FF7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Abram Liddell</t>
   </si>
@@ -124,6 +124,27 @@
   </si>
   <si>
     <t>At this point in time, the borders are able to generate with their respective parameters that allow passage through them without ending the game. The borders will not currently end the game, however, they'll just print "STATUS: Border Collision.". This is for ease of development purposes when testing other parts of the game so that it doesn't end quickly. Path generation has proved to be difficult. I know how to implement the mathematics required, but drawing the actual shape of the path is another job entirely. To complete this task as efficiently as possible willr require lots of trial and error to find the best method.</t>
+  </si>
+  <si>
+    <t>6/052021</t>
+  </si>
+  <si>
+    <t>Began designing background image on Pisekel</t>
+  </si>
+  <si>
+    <t>Background image design started on piskel. Planning to be a 700x300ish size, and take after a pixel neon city design.</t>
+  </si>
+  <si>
+    <t>Began testing multiprocessing</t>
+  </si>
+  <si>
+    <t>Came up with the idea of using multiprocessing as a way of creating the required path images without lagging the existing game. This makes use of parralel computing by using two cores instead of one, and limits the lagging which would normally be present if the game were to generate images as part of the normal script in one process.</t>
+  </si>
+  <si>
+    <t>Began implementing image generation for path generation.</t>
+  </si>
+  <si>
+    <t>Created base image to be rotated to a specified angle and cropped as per the automatic path generation process. The process also now runs parralel to the existing program, instead of inline and joining the current execution thread.</t>
   </si>
 </sst>
 </file>
@@ -166,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -181,7 +202,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -194,6 +215,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D95FED-742D-46A1-A295-BE0D9D7BF3DE}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:G15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -540,10 +564,10 @@
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="6"/>
@@ -728,7 +752,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="1">
-        <v>43892</v>
+        <v>44257</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>22</v>
@@ -745,7 +769,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="1">
-        <v>43893</v>
+        <v>44258</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>26</v>
@@ -762,7 +786,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="1">
-        <v>43894</v>
+        <v>44259</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>28</v>
@@ -773,128 +797,152 @@
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="9"/>
+      <c r="B17" s="3">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="9"/>
+      <c r="B18" s="5">
+        <v>14</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44323</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="9"/>
+      <c r="B19" s="5">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44326</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
-      <c r="B22" s="3"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -921,6 +969,10 @@
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="E26:G26"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="E10:G10"/>
@@ -931,11 +983,6 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="F2:G2"/>
     <mergeCell ref="A1:A30"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
@@ -951,6 +998,7 @@
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished path gen code: See logbook entry 16.
</commit_message>
<xml_diff>
--- a/Documentation/Logbook.xlsx
+++ b/Documentation/Logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abram\Documents\IT\Major Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC236C2-2E56-4759-8898-180B8EB765F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C0B313-65DF-4C20-A612-9252DA896477}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A4DA64FF-B9B3-4233-BC20-5B0DAEA49FF7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Abram Liddell</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Created base image to be rotated to a specified angle and cropped as per the automatic path generation process. The process also now runs parralel to the existing program, instead of inline and joining the current execution thread.</t>
+  </si>
+  <si>
+    <t>Finished path generation code</t>
+  </si>
+  <si>
+    <t>Fixed errors with path generation code and made it responsive to width limitations and angle limitaitons. Maybe at some point in the future, the width of the path itself may be implemented, but for now that's not important. This code now needs to be adapted to storing images in RAM to make the process faster, and it needs to be implemented into the existing game. It is currently a separate file.</t>
   </si>
 </sst>
 </file>
@@ -205,19 +211,19 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,7 +542,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -548,36 +554,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -587,14 +593,14 @@
       <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="3">
         <v>1</v>
       </c>
@@ -604,14 +610,14 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="3">
         <v>2</v>
       </c>
@@ -621,14 +627,14 @@
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="3">
         <v>3</v>
       </c>
@@ -638,14 +644,14 @@
       <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="3">
         <v>4</v>
       </c>
@@ -655,14 +661,14 @@
       <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="3">
         <v>5</v>
       </c>
@@ -672,14 +678,14 @@
       <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="3">
         <v>6</v>
       </c>
@@ -689,14 +695,14 @@
       <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="3">
         <v>7</v>
       </c>
@@ -706,14 +712,14 @@
       <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="3">
         <v>8</v>
       </c>
@@ -723,14 +729,14 @@
       <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="3">
         <v>9</v>
       </c>
@@ -740,14 +746,14 @@
       <c r="D13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="3">
         <v>10</v>
       </c>
@@ -757,14 +763,14 @@
       <c r="D14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="3">
         <v>11</v>
       </c>
@@ -774,14 +780,14 @@
       <c r="D15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" ht="87" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="4">
         <v>12</v>
       </c>
@@ -791,14 +797,14 @@
       <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="3">
         <v>13</v>
       </c>
@@ -808,14 +814,14 @@
       <c r="D17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="5">
         <v>14</v>
       </c>
@@ -825,14 +831,14 @@
       <c r="D18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="43" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="5">
         <v>15</v>
       </c>
@@ -842,147 +848,136 @@
       <c r="D19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7"/>
+      <c r="B20" s="5">
+        <v>16</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44337</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="5"/>
       <c r="C21" s="1"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="5"/>
       <c r="C22" s="1"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="5"/>
       <c r="C23" s="1"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="6"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="6"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="6"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="6"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.35">
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E23:G23"/>
     <mergeCell ref="A1:A30"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
@@ -999,6 +994,25 @@
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>